<commit_message>
add preview in datasets
</commit_message>
<xml_diff>
--- a/wdc_libs/ssechnpp-utils/!SEEChNPP_data_dictionary.xlsx
+++ b/wdc_libs/ssechnpp-utils/!SEEChNPP_data_dictionary.xlsx
@@ -2686,21 +2686,6 @@
     <t>./api/resource/Ch test-NSI.ico</t>
   </si>
   <si>
-    <t>./api/resource/undefined-control_unit.png</t>
-  </si>
-  <si>
-    <t>./api/resource/Ch test-radiation.png</t>
-  </si>
-  <si>
-    <t>./api/resource/Ch test-aerosole.png</t>
-  </si>
-  <si>
-    <t>./api/resource/Ch test-angle.png</t>
-  </si>
-  <si>
-    <t>./api/resource/Ch test-room.png</t>
-  </si>
-  <si>
     <t>Приміщення № Г-109-3</t>
   </si>
   <si>
@@ -2755,15 +2740,6 @@
     <t>Помещение № Г-107</t>
   </si>
   <si>
-    <t>./api/resource/Ch test-location.png</t>
-  </si>
-  <si>
-    <t>./api/resource/Ch test-well_unit.png</t>
-  </si>
-  <si>
-    <t>./api/resource/Ch test-axis.png</t>
-  </si>
-  <si>
     <t>#Set_label.lable</t>
   </si>
   <si>
@@ -3329,6 +3305,30 @@
   </si>
   <si>
     <t>Обьемная концентрация радиоактивных аэрозолей ß-типа в ЛЗ</t>
+  </si>
+  <si>
+    <t>./img/ssechnpp/aerosole.png</t>
+  </si>
+  <si>
+    <t>./img/ssechnpp/angle.png</t>
+  </si>
+  <si>
+    <t>./img/ssechnpp/room.png</t>
+  </si>
+  <si>
+    <t>./img/ssechnpp/location.png</t>
+  </si>
+  <si>
+    <t>./img/ssechnpp/axis.png</t>
+  </si>
+  <si>
+    <t>./img/ssechnpp/radiation.png</t>
+  </si>
+  <si>
+    <t>./img/ssechnpp/well-unit.png</t>
+  </si>
+  <si>
+    <t>./img/ssechnpp/control-unit.png</t>
   </si>
 </sst>
 </file>
@@ -3710,7 +3710,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5655,8 +5655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D417"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
-      <selection activeCell="B292" sqref="B292:D292"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6152,13 +6152,13 @@
         <v>42</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>842</v>
+        <v>1056</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>842</v>
+        <v>1056</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>842</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -6199,13 +6199,13 @@
         <v>47</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>842</v>
+        <v>1056</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>842</v>
+        <v>1056</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>842</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -6255,13 +6255,13 @@
         <v>52</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>842</v>
+        <v>1056</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>842</v>
+        <v>1056</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>842</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -6305,13 +6305,13 @@
         <v>57</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>842</v>
+        <v>1056</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>842</v>
+        <v>1056</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>842</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -6361,13 +6361,13 @@
         <v>62</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>843</v>
+        <v>1054</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>843</v>
+        <v>1054</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>843</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="105" x14ac:dyDescent="0.25">
@@ -6417,13 +6417,13 @@
         <v>67</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>843</v>
+        <v>1054</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>843</v>
+        <v>1054</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>843</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -6464,13 +6464,13 @@
         <v>831</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>844</v>
+        <v>1049</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>844</v>
+        <v>1049</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>844</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -6502,13 +6502,13 @@
         <v>830</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>844</v>
+        <v>1049</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>844</v>
+        <v>1049</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>844</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -6540,13 +6540,13 @@
         <v>80</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>845</v>
+        <v>1050</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>845</v>
+        <v>1050</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>845</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -6578,13 +6578,13 @@
         <v>85</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>845</v>
+        <v>1050</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>845</v>
+        <v>1050</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>845</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -6616,13 +6616,13 @@
         <v>90</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -6654,13 +6654,13 @@
         <v>95</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -6692,13 +6692,13 @@
         <v>100</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -6730,13 +6730,13 @@
         <v>105</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -6768,13 +6768,13 @@
         <v>110</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -6806,13 +6806,13 @@
         <v>115</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -6844,13 +6844,13 @@
         <v>120</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -6882,13 +6882,13 @@
         <v>125</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -6920,13 +6920,13 @@
         <v>130</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -6958,13 +6958,13 @@
         <v>135</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -6996,13 +6996,13 @@
         <v>140</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -7034,13 +7034,13 @@
         <v>145</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -7072,13 +7072,13 @@
         <v>150</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -7110,13 +7110,13 @@
         <v>155</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -7148,13 +7148,13 @@
         <v>160</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -7186,13 +7186,13 @@
         <v>165</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -7224,13 +7224,13 @@
         <v>170</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -7262,13 +7262,13 @@
         <v>175</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -7300,13 +7300,13 @@
         <v>180</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -7338,13 +7338,13 @@
         <v>185</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -7376,13 +7376,13 @@
         <v>190</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D156" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -7414,13 +7414,13 @@
         <v>195</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -7452,13 +7452,13 @@
         <v>200</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -7490,13 +7490,13 @@
         <v>205</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -7528,13 +7528,13 @@
         <v>210</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D172" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -7566,13 +7566,13 @@
         <v>215</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D176" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -7604,13 +7604,13 @@
         <v>220</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D180" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -7626,10 +7626,10 @@
         <v>550</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>847</v>
+        <v>842</v>
       </c>
       <c r="D182" s="4" t="s">
-        <v>849</v>
+        <v>844</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -7642,13 +7642,13 @@
         <v>225</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D184" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -7664,10 +7664,10 @@
         <v>551</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>848</v>
+        <v>843</v>
       </c>
       <c r="D186" s="4" t="s">
-        <v>850</v>
+        <v>845</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -7680,13 +7680,13 @@
         <v>230</v>
       </c>
       <c r="B188" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
       <c r="D188" s="4" t="s">
-        <v>846</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -7702,10 +7702,10 @@
         <v>552</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>851</v>
+        <v>846</v>
       </c>
       <c r="D190" s="4" t="s">
-        <v>854</v>
+        <v>849</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -7718,13 +7718,13 @@
         <v>235</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
       <c r="D192" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -7740,10 +7740,10 @@
         <v>553</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>852</v>
+        <v>847</v>
       </c>
       <c r="D194" s="4" t="s">
-        <v>855</v>
+        <v>850</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -7756,13 +7756,13 @@
         <v>240</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
       <c r="D196" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -7778,10 +7778,10 @@
         <v>554</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>853</v>
+        <v>848</v>
       </c>
       <c r="D198" s="4" t="s">
-        <v>856</v>
+        <v>851</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -7794,13 +7794,13 @@
         <v>245</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
       <c r="D200" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -7832,13 +7832,13 @@
         <v>250</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
       <c r="D204" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -7854,10 +7854,10 @@
         <v>558</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>857</v>
+        <v>852</v>
       </c>
       <c r="D206" s="4" t="s">
-        <v>858</v>
+        <v>853</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -7870,13 +7870,13 @@
         <v>255</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
       <c r="D208" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -7892,10 +7892,10 @@
         <v>559</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>859</v>
+        <v>854</v>
       </c>
       <c r="D210" s="4" t="s">
-        <v>860</v>
+        <v>855</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -7908,13 +7908,13 @@
         <v>260</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
       <c r="D212" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -7930,10 +7930,10 @@
         <v>560</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>861</v>
+        <v>856</v>
       </c>
       <c r="D214" s="4" t="s">
-        <v>862</v>
+        <v>857</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -7946,13 +7946,13 @@
         <v>265</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
       <c r="D216" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -7968,10 +7968,10 @@
         <v>561</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>863</v>
+        <v>858</v>
       </c>
       <c r="D218" s="4" t="s">
-        <v>864</v>
+        <v>859</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -7984,13 +7984,13 @@
         <v>270</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
       <c r="D220" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -8022,13 +8022,13 @@
         <v>275</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
       <c r="C224" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
       <c r="D224" s="4" t="s">
-        <v>865</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -8060,13 +8060,13 @@
         <v>280</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>866</v>
+        <v>1055</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>866</v>
+        <v>1055</v>
       </c>
       <c r="D228" s="4" t="s">
-        <v>866</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
@@ -8098,13 +8098,13 @@
         <v>285</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>866</v>
+        <v>1055</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>866</v>
+        <v>1055</v>
       </c>
       <c r="D232" s="4" t="s">
-        <v>866</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
@@ -8136,13 +8136,13 @@
         <v>290</v>
       </c>
       <c r="B236" s="4" t="s">
-        <v>866</v>
+        <v>1055</v>
       </c>
       <c r="C236" s="4" t="s">
-        <v>866</v>
+        <v>1055</v>
       </c>
       <c r="D236" s="4" t="s">
-        <v>866</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -8174,13 +8174,13 @@
         <v>295</v>
       </c>
       <c r="B240" s="4" t="s">
-        <v>866</v>
+        <v>1055</v>
       </c>
       <c r="C240" s="4" t="s">
-        <v>866</v>
+        <v>1055</v>
       </c>
       <c r="D240" s="4" t="s">
-        <v>866</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -8212,13 +8212,13 @@
         <v>300</v>
       </c>
       <c r="B244" s="4" t="s">
-        <v>866</v>
+        <v>1055</v>
       </c>
       <c r="C244" s="4" t="s">
-        <v>866</v>
+        <v>1055</v>
       </c>
       <c r="D244" s="4" t="s">
-        <v>866</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -8250,13 +8250,13 @@
         <v>305</v>
       </c>
       <c r="B248" s="4" t="s">
-        <v>866</v>
+        <v>1055</v>
       </c>
       <c r="C248" s="4" t="s">
-        <v>866</v>
+        <v>1055</v>
       </c>
       <c r="D248" s="4" t="s">
-        <v>866</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -8288,13 +8288,13 @@
         <v>310</v>
       </c>
       <c r="B252" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="D252" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
@@ -8326,13 +8326,13 @@
         <v>315</v>
       </c>
       <c r="B256" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="C256" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="D256" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
@@ -8364,13 +8364,13 @@
         <v>320</v>
       </c>
       <c r="B260" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="C260" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="D260" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
@@ -8402,13 +8402,13 @@
         <v>325</v>
       </c>
       <c r="B264" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="C264" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="D264" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
@@ -8440,13 +8440,13 @@
         <v>330</v>
       </c>
       <c r="B268" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="C268" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="D268" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
@@ -8478,13 +8478,13 @@
         <v>335</v>
       </c>
       <c r="B272" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="C272" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="D272" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
@@ -8516,13 +8516,13 @@
         <v>340</v>
       </c>
       <c r="B276" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="C276" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="D276" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
@@ -8554,13 +8554,13 @@
         <v>345</v>
       </c>
       <c r="B280" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="C280" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="D280" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
@@ -8592,13 +8592,13 @@
         <v>350</v>
       </c>
       <c r="B284" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="C284" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="D284" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
@@ -8630,13 +8630,13 @@
         <v>355</v>
       </c>
       <c r="B288" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="C288" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
       <c r="D288" s="4" t="s">
-        <v>867</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
@@ -8677,13 +8677,13 @@
         <v>360</v>
       </c>
       <c r="B292" s="4" t="s">
-        <v>843</v>
+        <v>1054</v>
       </c>
       <c r="C292" s="4" t="s">
-        <v>843</v>
+        <v>1054</v>
       </c>
       <c r="D292" s="4" t="s">
-        <v>843</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
@@ -8724,13 +8724,13 @@
         <v>365</v>
       </c>
       <c r="B296" s="4" t="s">
-        <v>843</v>
+        <v>1054</v>
       </c>
       <c r="C296" s="4" t="s">
-        <v>843</v>
+        <v>1054</v>
       </c>
       <c r="D296" s="4" t="s">
-        <v>843</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
@@ -8771,13 +8771,13 @@
         <v>370</v>
       </c>
       <c r="B300" s="4" t="s">
-        <v>844</v>
+        <v>1049</v>
       </c>
       <c r="C300" s="4" t="s">
-        <v>844</v>
+        <v>1049</v>
       </c>
       <c r="D300" s="4" t="s">
-        <v>844</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
@@ -8818,13 +8818,13 @@
         <v>375</v>
       </c>
       <c r="B304" s="4" t="s">
-        <v>844</v>
+        <v>1049</v>
       </c>
       <c r="C304" s="4" t="s">
-        <v>844</v>
+        <v>1049</v>
       </c>
       <c r="D304" s="4" t="s">
-        <v>844</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
@@ -8865,13 +8865,13 @@
         <v>380</v>
       </c>
       <c r="B308" s="4" t="s">
-        <v>845</v>
+        <v>1050</v>
       </c>
       <c r="C308" s="4" t="s">
-        <v>845</v>
+        <v>1050</v>
       </c>
       <c r="D308" s="4" t="s">
-        <v>845</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
@@ -8894,13 +8894,13 @@
         <v>385</v>
       </c>
       <c r="B312" s="4" t="s">
-        <v>845</v>
+        <v>1050</v>
       </c>
       <c r="C312" s="4" t="s">
-        <v>845</v>
+        <v>1050</v>
       </c>
       <c r="D312" s="4" t="s">
-        <v>845</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
@@ -8939,7 +8939,7 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" s="2" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="B318" s="4" t="s">
         <v>736</v>
@@ -8953,17 +8953,17 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
-        <v>869</v>
+        <v>861</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
-        <v>871</v>
+        <v>863</v>
       </c>
     </row>
     <row r="322" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -8981,13 +8981,13 @@
         <v>739</v>
       </c>
       <c r="B324" s="10" t="s">
-        <v>872</v>
+        <v>864</v>
       </c>
       <c r="C324" s="10" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="D324" s="10" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
     </row>
     <row r="325" spans="1:4" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -8995,13 +8995,13 @@
         <v>740</v>
       </c>
       <c r="B325" s="10" t="s">
-        <v>875</v>
+        <v>867</v>
       </c>
       <c r="C325" s="10" t="s">
-        <v>876</v>
+        <v>868</v>
       </c>
       <c r="D325" s="10" t="s">
-        <v>930</v>
+        <v>922</v>
       </c>
     </row>
     <row r="326" spans="1:4" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -9009,13 +9009,13 @@
         <v>741</v>
       </c>
       <c r="B326" s="10" t="s">
-        <v>877</v>
+        <v>869</v>
       </c>
       <c r="C326" s="10" t="s">
-        <v>878</v>
+        <v>870</v>
       </c>
       <c r="D326" s="10" t="s">
-        <v>879</v>
+        <v>871</v>
       </c>
     </row>
     <row r="327" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -9023,13 +9023,13 @@
         <v>742</v>
       </c>
       <c r="B327" s="10" t="s">
-        <v>880</v>
+        <v>872</v>
       </c>
       <c r="C327" s="10" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="D327" s="10" t="s">
-        <v>882</v>
+        <v>874</v>
       </c>
     </row>
     <row r="328" spans="1:4" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -9037,13 +9037,13 @@
         <v>743</v>
       </c>
       <c r="B328" s="10" t="s">
-        <v>883</v>
+        <v>875</v>
       </c>
       <c r="C328" s="10" t="s">
-        <v>884</v>
+        <v>876</v>
       </c>
       <c r="D328" s="10" t="s">
-        <v>885</v>
+        <v>877</v>
       </c>
     </row>
     <row r="329" spans="1:4" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -9051,13 +9051,13 @@
         <v>744</v>
       </c>
       <c r="B329" s="10" t="s">
-        <v>886</v>
+        <v>878</v>
       </c>
       <c r="C329" s="10" t="s">
-        <v>887</v>
+        <v>879</v>
       </c>
       <c r="D329" s="10" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
     </row>
     <row r="330" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -9075,13 +9075,13 @@
         <v>745</v>
       </c>
       <c r="B332" s="4" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
       <c r="C332" s="4" t="s">
-        <v>895</v>
+        <v>887</v>
       </c>
       <c r="D332" s="4" t="s">
-        <v>901</v>
+        <v>893</v>
       </c>
     </row>
     <row r="333" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9089,13 +9089,13 @@
         <v>746</v>
       </c>
       <c r="B333" s="4" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="C333" s="4" t="s">
-        <v>896</v>
+        <v>888</v>
       </c>
       <c r="D333" s="4" t="s">
-        <v>929</v>
+        <v>921</v>
       </c>
     </row>
     <row r="334" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9103,13 +9103,13 @@
         <v>747</v>
       </c>
       <c r="B334" s="4" t="s">
-        <v>891</v>
+        <v>883</v>
       </c>
       <c r="C334" s="4" t="s">
-        <v>897</v>
+        <v>889</v>
       </c>
       <c r="D334" s="4" t="s">
-        <v>902</v>
+        <v>894</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
@@ -9117,13 +9117,13 @@
         <v>748</v>
       </c>
       <c r="B335" s="4" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
       <c r="C335" s="4" t="s">
-        <v>898</v>
+        <v>890</v>
       </c>
       <c r="D335" s="4" t="s">
-        <v>903</v>
+        <v>895</v>
       </c>
     </row>
     <row r="336" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9131,13 +9131,13 @@
         <v>749</v>
       </c>
       <c r="B336" s="4" t="s">
-        <v>893</v>
+        <v>885</v>
       </c>
       <c r="C336" s="4" t="s">
-        <v>899</v>
+        <v>891</v>
       </c>
       <c r="D336" s="4" t="s">
-        <v>904</v>
+        <v>896</v>
       </c>
     </row>
     <row r="337" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9145,13 +9145,13 @@
         <v>750</v>
       </c>
       <c r="B337" s="4" t="s">
-        <v>894</v>
+        <v>886</v>
       </c>
       <c r="C337" s="4" t="s">
-        <v>900</v>
+        <v>892</v>
       </c>
       <c r="D337" s="4" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
     </row>
     <row r="338" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -9169,13 +9169,13 @@
         <v>754</v>
       </c>
       <c r="B340" s="4" t="s">
+        <v>898</v>
+      </c>
+      <c r="C340" s="4" t="s">
+        <v>902</v>
+      </c>
+      <c r="D340" s="4" t="s">
         <v>906</v>
-      </c>
-      <c r="C340" s="4" t="s">
-        <v>910</v>
-      </c>
-      <c r="D340" s="4" t="s">
-        <v>914</v>
       </c>
     </row>
     <row r="341" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9183,13 +9183,13 @@
         <v>755</v>
       </c>
       <c r="B341" s="4" t="s">
+        <v>899</v>
+      </c>
+      <c r="C341" s="4" t="s">
+        <v>903</v>
+      </c>
+      <c r="D341" s="4" t="s">
         <v>907</v>
-      </c>
-      <c r="C341" s="4" t="s">
-        <v>911</v>
-      </c>
-      <c r="D341" s="4" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="342" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9197,13 +9197,13 @@
         <v>756</v>
       </c>
       <c r="B342" s="4" t="s">
+        <v>900</v>
+      </c>
+      <c r="C342" s="4" t="s">
+        <v>904</v>
+      </c>
+      <c r="D342" s="4" t="s">
         <v>908</v>
-      </c>
-      <c r="C342" s="4" t="s">
-        <v>912</v>
-      </c>
-      <c r="D342" s="4" t="s">
-        <v>916</v>
       </c>
     </row>
     <row r="343" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9211,13 +9211,13 @@
         <v>757</v>
       </c>
       <c r="B343" s="4" t="s">
+        <v>901</v>
+      </c>
+      <c r="C343" s="4" t="s">
+        <v>905</v>
+      </c>
+      <c r="D343" s="4" t="s">
         <v>909</v>
-      </c>
-      <c r="C343" s="4" t="s">
-        <v>913</v>
-      </c>
-      <c r="D343" s="4" t="s">
-        <v>917</v>
       </c>
     </row>
     <row r="344" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9225,13 +9225,13 @@
         <v>758</v>
       </c>
       <c r="B344" s="4" t="s">
+        <v>901</v>
+      </c>
+      <c r="C344" s="4" t="s">
+        <v>905</v>
+      </c>
+      <c r="D344" s="4" t="s">
         <v>909</v>
-      </c>
-      <c r="C344" s="4" t="s">
-        <v>913</v>
-      </c>
-      <c r="D344" s="4" t="s">
-        <v>917</v>
       </c>
     </row>
     <row r="345" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9239,13 +9239,13 @@
         <v>759</v>
       </c>
       <c r="B345" s="4" t="s">
+        <v>901</v>
+      </c>
+      <c r="C345" s="4" t="s">
+        <v>905</v>
+      </c>
+      <c r="D345" s="4" t="s">
         <v>909</v>
-      </c>
-      <c r="C345" s="4" t="s">
-        <v>913</v>
-      </c>
-      <c r="D345" s="4" t="s">
-        <v>917</v>
       </c>
     </row>
     <row r="346" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9253,13 +9253,13 @@
         <v>760</v>
       </c>
       <c r="B346" s="4" t="s">
+        <v>901</v>
+      </c>
+      <c r="C346" s="4" t="s">
+        <v>905</v>
+      </c>
+      <c r="D346" s="4" t="s">
         <v>909</v>
-      </c>
-      <c r="C346" s="4" t="s">
-        <v>913</v>
-      </c>
-      <c r="D346" s="4" t="s">
-        <v>917</v>
       </c>
     </row>
     <row r="347" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -9277,13 +9277,13 @@
         <v>762</v>
       </c>
       <c r="B349" s="4" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="C349" s="4" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
       <c r="D349" s="4" t="s">
-        <v>920</v>
+        <v>912</v>
       </c>
     </row>
     <row r="350" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9291,13 +9291,13 @@
         <v>763</v>
       </c>
       <c r="B350" s="4" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="C350" s="4" t="s">
-        <v>922</v>
+        <v>914</v>
       </c>
       <c r="D350" s="4" t="s">
-        <v>923</v>
+        <v>915</v>
       </c>
     </row>
     <row r="351" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9305,13 +9305,13 @@
         <v>764</v>
       </c>
       <c r="B351" s="4" t="s">
-        <v>924</v>
+        <v>916</v>
       </c>
       <c r="C351" s="4" t="s">
-        <v>925</v>
+        <v>917</v>
       </c>
       <c r="D351" s="4" t="s">
-        <v>926</v>
+        <v>918</v>
       </c>
     </row>
     <row r="352" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9319,13 +9319,13 @@
         <v>765</v>
       </c>
       <c r="B352" s="4" t="s">
-        <v>927</v>
+        <v>919</v>
       </c>
       <c r="C352" s="4" t="s">
-        <v>928</v>
+        <v>920</v>
       </c>
       <c r="D352" s="4" t="s">
-        <v>1056</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="353" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9333,13 +9333,13 @@
         <v>766</v>
       </c>
       <c r="B353" s="4" t="s">
-        <v>927</v>
+        <v>919</v>
       </c>
       <c r="C353" s="4" t="s">
-        <v>928</v>
+        <v>920</v>
       </c>
       <c r="D353" s="4" t="s">
-        <v>1056</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="354" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9347,13 +9347,13 @@
         <v>767</v>
       </c>
       <c r="B354" s="4" t="s">
-        <v>927</v>
+        <v>919</v>
       </c>
       <c r="C354" s="4" t="s">
-        <v>928</v>
+        <v>920</v>
       </c>
       <c r="D354" s="4" t="s">
-        <v>1056</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="355" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9361,13 +9361,13 @@
         <v>768</v>
       </c>
       <c r="B355" s="4" t="s">
-        <v>927</v>
+        <v>919</v>
       </c>
       <c r="C355" s="4" t="s">
-        <v>928</v>
+        <v>920</v>
       </c>
       <c r="D355" s="4" t="s">
-        <v>1056</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="356" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -9385,13 +9385,13 @@
         <v>770</v>
       </c>
       <c r="B358" s="10" t="s">
-        <v>931</v>
+        <v>923</v>
       </c>
       <c r="C358" s="10" t="s">
-        <v>932</v>
+        <v>924</v>
       </c>
       <c r="D358" s="10" t="s">
-        <v>933</v>
+        <v>925</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
@@ -9399,13 +9399,13 @@
         <v>771</v>
       </c>
       <c r="B359" s="10" t="s">
-        <v>931</v>
+        <v>923</v>
       </c>
       <c r="C359" s="10" t="s">
-        <v>932</v>
+        <v>924</v>
       </c>
       <c r="D359" s="10" t="s">
-        <v>933</v>
+        <v>925</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
@@ -9413,13 +9413,13 @@
         <v>772</v>
       </c>
       <c r="B360" s="10" t="s">
-        <v>931</v>
+        <v>923</v>
       </c>
       <c r="C360" s="10" t="s">
-        <v>932</v>
+        <v>924</v>
       </c>
       <c r="D360" s="10" t="s">
-        <v>933</v>
+        <v>925</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
@@ -9427,13 +9427,13 @@
         <v>773</v>
       </c>
       <c r="B361" s="10" t="s">
-        <v>931</v>
+        <v>923</v>
       </c>
       <c r="C361" s="10" t="s">
-        <v>932</v>
+        <v>924</v>
       </c>
       <c r="D361" s="10" t="s">
-        <v>933</v>
+        <v>925</v>
       </c>
     </row>
     <row r="362" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -9451,13 +9451,13 @@
         <v>774</v>
       </c>
       <c r="B364" s="10" t="s">
-        <v>934</v>
+        <v>926</v>
       </c>
       <c r="C364" s="10" t="s">
-        <v>936</v>
+        <v>928</v>
       </c>
       <c r="D364" s="10" t="s">
-        <v>935</v>
+        <v>927</v>
       </c>
     </row>
     <row r="365" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9465,13 +9465,13 @@
         <v>775</v>
       </c>
       <c r="B365" s="10" t="s">
-        <v>937</v>
+        <v>929</v>
       </c>
       <c r="C365" s="10" t="s">
-        <v>939</v>
+        <v>931</v>
       </c>
       <c r="D365" s="10" t="s">
-        <v>938</v>
+        <v>930</v>
       </c>
     </row>
     <row r="366" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9479,13 +9479,13 @@
         <v>776</v>
       </c>
       <c r="B366" s="10" t="s">
-        <v>940</v>
+        <v>932</v>
       </c>
       <c r="C366" s="10" t="s">
-        <v>941</v>
+        <v>933</v>
       </c>
       <c r="D366" s="10" t="s">
-        <v>942</v>
+        <v>934</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
@@ -9493,13 +9493,13 @@
         <v>777</v>
       </c>
       <c r="B367" s="10" t="s">
-        <v>943</v>
+        <v>935</v>
       </c>
       <c r="C367" s="10" t="s">
-        <v>956</v>
+        <v>948</v>
       </c>
       <c r="D367" s="10" t="s">
-        <v>957</v>
+        <v>949</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
@@ -9507,13 +9507,13 @@
         <v>778</v>
       </c>
       <c r="B368" s="10" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="C368" s="10" t="s">
-        <v>945</v>
+        <v>937</v>
       </c>
       <c r="D368" s="10" t="s">
-        <v>946</v>
+        <v>938</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
@@ -9521,13 +9521,13 @@
         <v>779</v>
       </c>
       <c r="B369" s="10" t="s">
-        <v>947</v>
+        <v>939</v>
       </c>
       <c r="C369" s="10" t="s">
-        <v>948</v>
+        <v>940</v>
       </c>
       <c r="D369" s="10" t="s">
-        <v>949</v>
+        <v>941</v>
       </c>
     </row>
     <row r="370" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9535,13 +9535,13 @@
         <v>780</v>
       </c>
       <c r="B370" s="10" t="s">
-        <v>950</v>
+        <v>942</v>
       </c>
       <c r="C370" s="10" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="D370" s="10" t="s">
-        <v>954</v>
+        <v>946</v>
       </c>
     </row>
     <row r="371" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9549,13 +9549,13 @@
         <v>781</v>
       </c>
       <c r="B371" s="10" t="s">
-        <v>951</v>
+        <v>943</v>
       </c>
       <c r="C371" s="10" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="D371" s="10" t="s">
-        <v>955</v>
+        <v>947</v>
       </c>
     </row>
     <row r="372" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -9573,13 +9573,13 @@
         <v>782</v>
       </c>
       <c r="B374" s="4" t="s">
-        <v>958</v>
+        <v>950</v>
       </c>
       <c r="C374" s="4" t="s">
-        <v>959</v>
+        <v>951</v>
       </c>
       <c r="D374" s="4" t="s">
-        <v>960</v>
+        <v>952</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
@@ -9587,13 +9587,13 @@
         <v>783</v>
       </c>
       <c r="B375" s="4" t="s">
-        <v>961</v>
+        <v>953</v>
       </c>
       <c r="C375" s="4" t="s">
-        <v>962</v>
+        <v>954</v>
       </c>
       <c r="D375" s="4" t="s">
-        <v>963</v>
+        <v>955</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
@@ -9601,13 +9601,13 @@
         <v>784</v>
       </c>
       <c r="B376" s="4" t="s">
-        <v>964</v>
+        <v>956</v>
       </c>
       <c r="C376" s="4" t="s">
-        <v>965</v>
+        <v>957</v>
       </c>
       <c r="D376" s="4" t="s">
-        <v>966</v>
+        <v>958</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
@@ -9615,13 +9615,13 @@
         <v>785</v>
       </c>
       <c r="B377" s="4" t="s">
-        <v>967</v>
+        <v>959</v>
       </c>
       <c r="C377" s="4" t="s">
-        <v>968</v>
+        <v>960</v>
       </c>
       <c r="D377" s="4" t="s">
-        <v>969</v>
+        <v>961</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
@@ -9629,13 +9629,13 @@
         <v>786</v>
       </c>
       <c r="B378" s="4" t="s">
-        <v>970</v>
+        <v>962</v>
       </c>
       <c r="C378" s="4" t="s">
-        <v>971</v>
+        <v>963</v>
       </c>
       <c r="D378" s="4" t="s">
-        <v>972</v>
+        <v>964</v>
       </c>
     </row>
     <row r="379" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -9653,13 +9653,13 @@
         <v>787</v>
       </c>
       <c r="B381" s="4" t="s">
-        <v>973</v>
+        <v>965</v>
       </c>
       <c r="C381" s="4" t="s">
-        <v>974</v>
+        <v>966</v>
       </c>
       <c r="D381" s="4" t="s">
-        <v>975</v>
+        <v>967</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
@@ -9667,13 +9667,13 @@
         <v>788</v>
       </c>
       <c r="B382" s="4" t="s">
-        <v>976</v>
+        <v>968</v>
       </c>
       <c r="C382" s="4" t="s">
-        <v>977</v>
+        <v>969</v>
       </c>
       <c r="D382" s="4" t="s">
-        <v>978</v>
+        <v>970</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
@@ -9681,13 +9681,13 @@
         <v>789</v>
       </c>
       <c r="B383" s="4" t="s">
-        <v>979</v>
+        <v>971</v>
       </c>
       <c r="C383" s="4" t="s">
-        <v>980</v>
+        <v>972</v>
       </c>
       <c r="D383" s="4" t="s">
-        <v>981</v>
+        <v>973</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
@@ -9695,13 +9695,13 @@
         <v>790</v>
       </c>
       <c r="B384" s="4" t="s">
-        <v>982</v>
+        <v>974</v>
       </c>
       <c r="C384" s="4" t="s">
-        <v>983</v>
+        <v>975</v>
       </c>
       <c r="D384" s="4" t="s">
-        <v>984</v>
+        <v>976</v>
       </c>
     </row>
     <row r="385" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -9719,13 +9719,13 @@
         <v>791</v>
       </c>
       <c r="B387" s="4" t="s">
-        <v>986</v>
+        <v>978</v>
       </c>
       <c r="C387" s="4" t="s">
-        <v>991</v>
+        <v>983</v>
       </c>
       <c r="D387" s="4" t="s">
-        <v>996</v>
+        <v>988</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
@@ -9733,13 +9733,13 @@
         <v>792</v>
       </c>
       <c r="B388" s="4" t="s">
-        <v>987</v>
+        <v>979</v>
       </c>
       <c r="C388" s="4" t="s">
-        <v>992</v>
+        <v>984</v>
       </c>
       <c r="D388" s="4" t="s">
-        <v>997</v>
+        <v>989</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
@@ -9747,13 +9747,13 @@
         <v>793</v>
       </c>
       <c r="B389" s="4" t="s">
-        <v>988</v>
+        <v>980</v>
       </c>
       <c r="C389" s="4" t="s">
-        <v>993</v>
+        <v>985</v>
       </c>
       <c r="D389" s="4" t="s">
-        <v>998</v>
+        <v>990</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
@@ -9761,13 +9761,13 @@
         <v>794</v>
       </c>
       <c r="B390" s="4" t="s">
-        <v>989</v>
+        <v>981</v>
       </c>
       <c r="C390" s="4" t="s">
-        <v>994</v>
+        <v>986</v>
       </c>
       <c r="D390" s="4" t="s">
-        <v>999</v>
+        <v>991</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
@@ -9775,13 +9775,13 @@
         <v>795</v>
       </c>
       <c r="B391" s="4" t="s">
-        <v>990</v>
+        <v>982</v>
       </c>
       <c r="C391" s="4" t="s">
-        <v>995</v>
+        <v>987</v>
       </c>
       <c r="D391" s="4" t="s">
-        <v>1000</v>
+        <v>992</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.25">
@@ -9789,7 +9789,7 @@
         <v>796</v>
       </c>
       <c r="B392" s="4" t="s">
-        <v>985</v>
+        <v>977</v>
       </c>
       <c r="C392" s="4" t="s">
         <v>476</v>
@@ -9813,13 +9813,13 @@
         <v>797</v>
       </c>
       <c r="B395" s="4" t="s">
+        <v>993</v>
+      </c>
+      <c r="C395" s="4" t="s">
         <v>1001</v>
       </c>
-      <c r="C395" s="4" t="s">
-        <v>1009</v>
-      </c>
       <c r="D395" s="4" t="s">
-        <v>1016</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.25">
@@ -9827,13 +9827,13 @@
         <v>798</v>
       </c>
       <c r="B396" s="4" t="s">
+        <v>994</v>
+      </c>
+      <c r="C396" s="4" t="s">
         <v>1002</v>
       </c>
-      <c r="C396" s="4" t="s">
-        <v>1010</v>
-      </c>
       <c r="D396" s="4" t="s">
-        <v>1017</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.25">
@@ -9841,13 +9841,13 @@
         <v>799</v>
       </c>
       <c r="B397" s="4" t="s">
+        <v>995</v>
+      </c>
+      <c r="C397" s="4" t="s">
         <v>1003</v>
       </c>
-      <c r="C397" s="4" t="s">
-        <v>1011</v>
-      </c>
       <c r="D397" s="4" t="s">
-        <v>1018</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="398" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9855,13 +9855,13 @@
         <v>800</v>
       </c>
       <c r="B398" s="10" t="s">
+        <v>996</v>
+      </c>
+      <c r="C398" s="10" t="s">
         <v>1004</v>
       </c>
-      <c r="C398" s="10" t="s">
+      <c r="D398" s="10" t="s">
         <v>1012</v>
-      </c>
-      <c r="D398" s="10" t="s">
-        <v>1020</v>
       </c>
     </row>
     <row r="399" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9869,13 +9869,13 @@
         <v>801</v>
       </c>
       <c r="B399" s="10" t="s">
+        <v>997</v>
+      </c>
+      <c r="C399" s="10" t="s">
         <v>1005</v>
       </c>
-      <c r="C399" s="10" t="s">
+      <c r="D399" s="10" t="s">
         <v>1013</v>
-      </c>
-      <c r="D399" s="10" t="s">
-        <v>1021</v>
       </c>
     </row>
     <row r="400" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9883,13 +9883,13 @@
         <v>802</v>
       </c>
       <c r="B400" s="10" t="s">
+        <v>998</v>
+      </c>
+      <c r="C400" s="10" t="s">
         <v>1006</v>
       </c>
-      <c r="C400" s="10" t="s">
+      <c r="D400" s="10" t="s">
         <v>1014</v>
-      </c>
-      <c r="D400" s="10" t="s">
-        <v>1022</v>
       </c>
     </row>
     <row r="401" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9897,13 +9897,13 @@
         <v>803</v>
       </c>
       <c r="B401" s="10" t="s">
-        <v>1007</v>
+        <v>999</v>
       </c>
       <c r="C401" s="10" t="s">
-        <v>1012</v>
+        <v>1004</v>
       </c>
       <c r="D401" s="10" t="s">
-        <v>1023</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.25">
@@ -9911,13 +9911,13 @@
         <v>804</v>
       </c>
       <c r="B402" s="4" t="s">
-        <v>1008</v>
+        <v>1000</v>
       </c>
       <c r="C402" s="4" t="s">
-        <v>1015</v>
+        <v>1007</v>
       </c>
       <c r="D402" s="10" t="s">
-        <v>1019</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="403" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -9935,13 +9935,13 @@
         <v>805</v>
       </c>
       <c r="B405" s="4" t="s">
-        <v>1024</v>
+        <v>1016</v>
       </c>
       <c r="C405" s="4" t="s">
-        <v>1027</v>
+        <v>1019</v>
       </c>
       <c r="D405" s="4" t="s">
-        <v>1030</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.25">
@@ -9949,13 +9949,13 @@
         <v>806</v>
       </c>
       <c r="B406" s="4" t="s">
-        <v>1025</v>
+        <v>1017</v>
       </c>
       <c r="C406" s="4" t="s">
-        <v>1028</v>
+        <v>1020</v>
       </c>
       <c r="D406" s="4" t="s">
-        <v>1029</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
@@ -9963,13 +9963,13 @@
         <v>807</v>
       </c>
       <c r="B407" s="4" t="s">
-        <v>1026</v>
+        <v>1018</v>
       </c>
       <c r="C407" s="4" t="s">
-        <v>1031</v>
+        <v>1023</v>
       </c>
       <c r="D407" s="4" t="s">
-        <v>1032</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="408" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -9984,72 +9984,72 @@
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A410" s="7" t="s">
-        <v>1033</v>
+        <v>1025</v>
       </c>
       <c r="B410" s="4" t="s">
-        <v>1038</v>
+        <v>1030</v>
       </c>
       <c r="C410" s="4" t="s">
-        <v>1043</v>
+        <v>1035</v>
       </c>
       <c r="D410" s="4" t="s">
-        <v>1048</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A411" s="7" t="s">
-        <v>1034</v>
+        <v>1026</v>
       </c>
       <c r="B411" s="4" t="s">
-        <v>1039</v>
+        <v>1031</v>
       </c>
       <c r="C411" s="4" t="s">
-        <v>1046</v>
+        <v>1038</v>
       </c>
       <c r="D411" s="4" t="s">
-        <v>1050</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A412" s="7" t="s">
-        <v>1035</v>
+        <v>1027</v>
       </c>
       <c r="B412" s="4" t="s">
-        <v>1040</v>
+        <v>1032</v>
       </c>
       <c r="C412" s="4" t="s">
-        <v>1047</v>
+        <v>1039</v>
       </c>
       <c r="D412" s="4" t="s">
-        <v>1051</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A413" s="7" t="s">
-        <v>1036</v>
+        <v>1028</v>
       </c>
       <c r="B413" s="4" t="s">
-        <v>1041</v>
+        <v>1033</v>
       </c>
       <c r="C413" s="4" t="s">
-        <v>1045</v>
+        <v>1037</v>
       </c>
       <c r="D413" s="4" t="s">
-        <v>1052</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A414" s="7" t="s">
-        <v>1037</v>
+        <v>1029</v>
       </c>
       <c r="B414" s="4" t="s">
-        <v>1042</v>
+        <v>1034</v>
       </c>
       <c r="C414" s="4" t="s">
-        <v>1044</v>
+        <v>1036</v>
       </c>
       <c r="D414" s="4" t="s">
-        <v>1049</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="415" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -10067,13 +10067,13 @@
         <v>810</v>
       </c>
       <c r="B417" s="4" t="s">
-        <v>1053</v>
+        <v>1045</v>
       </c>
       <c r="C417" s="4" t="s">
-        <v>1054</v>
+        <v>1046</v>
       </c>
       <c r="D417" s="4" t="s">
-        <v>1055</v>
+        <v>1047</v>
       </c>
     </row>
   </sheetData>

</xml_diff>